<commit_message>
Carla UPDATE LEAVE CARD 4/7/2023 7:41 PM
</commit_message>
<xml_diff>
--- a/ACERON, ANGELU.xlsx
+++ b/ACERON, ANGELU.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-44REB32\Users\ASUS\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1C1DEC-4ECC-4804-B331-7852B74F5973}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <definedName name="BALANCE_1">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>PERIOD</t>
   </si>
@@ -214,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -590,9 +591,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -602,17 +600,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -823,6 +824,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -830,12 +837,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -902,7 +903,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -945,7 +946,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1009,7 +1010,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1069,7 +1070,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1135,7 +1136,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1198,7 +1199,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1296,7 +1297,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1355,7 +1356,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,7 +1421,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1463,7 +1464,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1538,7 +1539,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1724,7 +1725,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1790,7 +1791,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1848,7 +1849,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1914,7 +1915,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1970,7 +1971,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2045,7 +2046,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2088,7 +2089,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2154,7 +2155,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2210,7 +2211,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2306,25 +2307,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K133" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K133" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2631,7 +2632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2641,7 +2642,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2649,99 +2650,99 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A10" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A16" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="55">
         <v>44594</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -2749,7 +2750,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -2762,24 +2763,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -2823,7 +2824,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>3.7080000000000002</v>
+        <v>6.2079999999999984</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2833,12 +2834,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>13.708</v>
+        <v>16.207999999999998</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>46</v>
       </c>
@@ -2860,7 +2861,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>44594</v>
       </c>
@@ -2880,7 +2881,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>44622</v>
       </c>
@@ -2900,7 +2901,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>44653</v>
       </c>
@@ -2920,7 +2921,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>44683</v>
       </c>
@@ -2940,7 +2941,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>44714</v>
       </c>
@@ -2960,7 +2961,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>44744</v>
       </c>
@@ -2980,7 +2981,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>44775</v>
       </c>
@@ -3000,7 +3001,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>44806</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40"/>
       <c r="B19" s="20"/>
       <c r="C19" s="13">
@@ -3040,7 +3041,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>44835</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>44866</v>
       </c>
@@ -3092,7 +3093,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
       <c r="B22" s="20" t="s">
         <v>52</v>
@@ -3114,7 +3115,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
         <v>44896</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
       <c r="B24" s="20" t="s">
         <v>56</v>
@@ -3158,7 +3159,7 @@
         <v>44918</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
       <c r="B25" s="20" t="s">
         <v>57</v>
@@ -3180,7 +3181,7 @@
         <v>44923</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
         <v>54</v>
       </c>
@@ -3198,7 +3199,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>44927</v>
       </c>
@@ -3218,45 +3219,53 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <f>EDATE(A27,1)</f>
         <v>44958</v>
       </c>
       <c r="B28" s="20"/>
-      <c r="C28" s="13"/>
+      <c r="C28" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D28" s="39"/>
       <c r="E28" s="9"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G28" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H28" s="39"/>
       <c r="I28" s="9"/>
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <f t="shared" ref="A29:A53" si="0">EDATE(A28,1)</f>
         <v>44986</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="13"/>
+      <c r="B29" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D29" s="39"/>
       <c r="E29" s="9"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G29" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H29" s="39"/>
       <c r="I29" s="9"/>
       <c r="J29" s="11"/>
-      <c r="K29" s="20"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="49">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <f t="shared" si="0"/>
         <v>45017</v>
@@ -3275,7 +3284,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <f t="shared" si="0"/>
         <v>45047</v>
@@ -3294,7 +3303,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <f t="shared" si="0"/>
         <v>45078</v>
@@ -3313,7 +3322,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <f t="shared" si="0"/>
         <v>45108</v>
@@ -3332,7 +3341,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <f t="shared" si="0"/>
         <v>45139</v>
@@ -3351,7 +3360,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <f t="shared" si="0"/>
         <v>45170</v>
@@ -3370,7 +3379,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="40">
         <f t="shared" si="0"/>
         <v>45200</v>
@@ -3389,7 +3398,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <f t="shared" si="0"/>
         <v>45231</v>
@@ -3408,7 +3417,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <f t="shared" si="0"/>
         <v>45261</v>
@@ -3427,7 +3436,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <f t="shared" si="0"/>
         <v>45292</v>
@@ -3446,7 +3455,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <f t="shared" si="0"/>
         <v>45323</v>
@@ -3465,7 +3474,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <f t="shared" si="0"/>
         <v>45352</v>
@@ -3484,7 +3493,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <f t="shared" si="0"/>
         <v>45383</v>
@@ -3503,7 +3512,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <f t="shared" si="0"/>
         <v>45413</v>
@@ -3522,7 +3531,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <f t="shared" si="0"/>
         <v>45444</v>
@@ -3541,7 +3550,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <f t="shared" si="0"/>
         <v>45474</v>
@@ -3560,7 +3569,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <f t="shared" si="0"/>
         <v>45505</v>
@@ -3579,7 +3588,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <f t="shared" si="0"/>
         <v>45536</v>
@@ -3598,7 +3607,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <f t="shared" si="0"/>
         <v>45566</v>
@@ -3617,7 +3626,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40">
         <f t="shared" si="0"/>
         <v>45597</v>
@@ -3636,7 +3645,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <f t="shared" si="0"/>
         <v>45627</v>
@@ -3655,7 +3664,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <f t="shared" si="0"/>
         <v>45658</v>
@@ -3674,7 +3683,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <f t="shared" si="0"/>
         <v>45689</v>
@@ -3693,7 +3702,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <f t="shared" si="0"/>
         <v>45717</v>
@@ -3712,7 +3721,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -3728,7 +3737,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -3744,7 +3753,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -3760,7 +3769,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -3776,7 +3785,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -3792,7 +3801,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -3808,7 +3817,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -3824,7 +3833,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -3840,7 +3849,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -3856,7 +3865,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -3872,7 +3881,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -3888,7 +3897,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -3904,7 +3913,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -3920,7 +3929,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -3936,7 +3945,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -3952,7 +3961,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -3968,7 +3977,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -3984,7 +3993,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -4000,7 +4009,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -4016,7 +4025,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -4032,7 +4041,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -4048,7 +4057,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4064,7 +4073,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4080,7 +4089,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4096,7 +4105,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4112,7 +4121,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4128,7 +4137,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4144,7 +4153,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4160,7 +4169,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4176,7 +4185,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4192,7 +4201,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4208,7 +4217,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4224,7 +4233,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4240,7 +4249,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4256,7 +4265,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4272,7 +4281,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4288,7 +4297,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4304,7 +4313,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4320,7 +4329,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4336,7 +4345,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4352,7 +4361,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4368,7 +4377,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4384,7 +4393,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4400,7 +4409,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4416,7 +4425,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4432,7 +4441,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4448,7 +4457,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4464,7 +4473,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4480,7 +4489,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4496,7 +4505,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4512,7 +4521,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4528,7 +4537,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4544,7 +4553,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4560,7 +4569,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4576,7 +4585,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4592,7 +4601,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4608,7 +4617,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4624,7 +4633,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4640,7 +4649,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4656,7 +4665,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4672,7 +4681,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4688,7 +4697,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4704,7 +4713,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4720,7 +4729,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4736,7 +4745,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4752,7 +4761,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4768,7 +4777,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -4784,7 +4793,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -4800,7 +4809,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -4816,7 +4825,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -4832,7 +4841,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -4848,7 +4857,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -4864,7 +4873,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -4880,7 +4889,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -4896,7 +4905,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -4912,7 +4921,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -4928,7 +4937,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -4944,7 +4953,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -4960,7 +4969,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -4976,7 +4985,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="41"/>
       <c r="B133" s="15"/>
       <c r="C133" s="42"/>
@@ -4994,23 +5003,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5033,28 +5042,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5067,7 +5076,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5096,7 +5105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3" s="11"/>
@@ -5118,17 +5127,17 @@
         <v>1.208</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5149,7 +5158,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5176,7 +5185,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5202,7 +5211,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5228,7 +5237,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5254,7 +5263,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5280,7 +5289,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5306,7 +5315,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5332,7 +5341,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5358,7 +5367,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5378,7 +5387,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5398,7 +5407,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5418,7 +5427,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5439,7 +5448,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5460,7 +5469,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5481,7 +5490,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5502,7 +5511,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5523,7 +5532,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5544,7 +5553,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -5565,7 +5574,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -5586,7 +5595,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -5607,7 +5616,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -5628,7 +5637,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -5649,7 +5658,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -5670,7 +5679,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -5691,7 +5700,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -5712,7 +5721,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -5733,7 +5742,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -5754,7 +5763,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -5775,7 +5784,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -5796,7 +5805,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -5817,7 +5826,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -5838,7 +5847,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -5847,7 +5856,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -5856,7 +5865,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -5865,7 +5874,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -5874,7 +5883,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -5883,7 +5892,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -5892,7 +5901,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -5901,7 +5910,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -5910,7 +5919,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -5919,7 +5928,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -5928,7 +5937,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -5937,7 +5946,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -5946,7 +5955,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -5955,7 +5964,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -5964,7 +5973,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -5973,7 +5982,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -5982,7 +5991,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -5991,7 +6000,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6000,7 +6009,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6009,7 +6018,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6018,7 +6027,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6027,7 +6036,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6036,7 +6045,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6045,7 +6054,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6054,7 +6063,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6063,7 +6072,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6072,7 +6081,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6081,7 +6090,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6090,7 +6099,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6099,7 +6108,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
Update Leave Card 4/12/2023 4:43 PM
</commit_message>
<xml_diff>
--- a/ACERON, ANGELU.xlsx
+++ b/ACERON, ANGELU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1C1DEC-4ECC-4804-B331-7852B74F5973}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D977A8C3-12E5-4264-8A9F-E3906E4B6942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>PERIOD</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>VL(1-0-0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -594,17 +597,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -614,6 +614,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2307,7 +2310,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K133" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K135" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="9"/>
@@ -2654,12 +2657,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K133"/>
+  <dimension ref="A2:K135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A16" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A25" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2689,14 +2692,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -2709,16 +2712,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>44594</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -2731,16 +2734,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -2766,18 +2769,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3242,7 +3245,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
-        <f t="shared" ref="A29:A53" si="0">EDATE(A28,1)</f>
+        <f t="shared" ref="A29:A55" si="0">EDATE(A28,1)</f>
         <v>44986</v>
       </c>
       <c r="B29" s="20" t="s">
@@ -3266,11 +3269,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="40">
-        <f t="shared" si="0"/>
-        <v>45017</v>
-      </c>
-      <c r="B30" s="20"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="C30" s="13"/>
       <c r="D30" s="39"/>
       <c r="E30" s="9"/>
@@ -3282,14 +3284,15 @@
       <c r="H30" s="39"/>
       <c r="I30" s="9"/>
       <c r="J30" s="11"/>
-      <c r="K30" s="20"/>
+      <c r="K30" s="49">
+        <v>45000</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="40">
-        <f t="shared" si="0"/>
-        <v>45047</v>
-      </c>
-      <c r="B31" s="20"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="C31" s="13"/>
       <c r="D31" s="39"/>
       <c r="E31" s="9"/>
@@ -3301,14 +3304,18 @@
       <c r="H31" s="39"/>
       <c r="I31" s="9"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="20"/>
+      <c r="K31" s="49">
+        <v>45013</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
-        <f t="shared" si="0"/>
-        <v>45078</v>
-      </c>
-      <c r="B32" s="20"/>
+        <f>EDATE(A29,1)</f>
+        <v>45017</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="C32" s="13"/>
       <c r="D32" s="39"/>
       <c r="E32" s="9"/>
@@ -3325,7 +3332,7 @@
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <f t="shared" si="0"/>
-        <v>45108</v>
+        <v>45047</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -3344,7 +3351,7 @@
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <f t="shared" si="0"/>
-        <v>45139</v>
+        <v>45078</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -3363,7 +3370,7 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <f t="shared" si="0"/>
-        <v>45170</v>
+        <v>45108</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -3382,7 +3389,7 @@
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="40">
         <f t="shared" si="0"/>
-        <v>45200</v>
+        <v>45139</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -3401,7 +3408,7 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <f t="shared" si="0"/>
-        <v>45231</v>
+        <v>45170</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -3420,7 +3427,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <f t="shared" si="0"/>
-        <v>45261</v>
+        <v>45200</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -3439,7 +3446,7 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <f t="shared" si="0"/>
-        <v>45292</v>
+        <v>45231</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -3458,7 +3465,7 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <f t="shared" si="0"/>
-        <v>45323</v>
+        <v>45261</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -3477,7 +3484,7 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <f t="shared" si="0"/>
-        <v>45352</v>
+        <v>45292</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -3496,7 +3503,7 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <f t="shared" si="0"/>
-        <v>45383</v>
+        <v>45323</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -3515,7 +3522,7 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <f t="shared" si="0"/>
-        <v>45413</v>
+        <v>45352</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -3534,7 +3541,7 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <f t="shared" si="0"/>
-        <v>45444</v>
+        <v>45383</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -3553,7 +3560,7 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <f t="shared" si="0"/>
-        <v>45474</v>
+        <v>45413</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -3572,7 +3579,7 @@
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <f t="shared" si="0"/>
-        <v>45505</v>
+        <v>45444</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -3591,7 +3598,7 @@
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <f t="shared" si="0"/>
-        <v>45536</v>
+        <v>45474</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -3610,7 +3617,7 @@
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <f t="shared" si="0"/>
-        <v>45566</v>
+        <v>45505</v>
       </c>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -3629,7 +3636,7 @@
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40">
         <f t="shared" si="0"/>
-        <v>45597</v>
+        <v>45536</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -3648,7 +3655,7 @@
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <f t="shared" si="0"/>
-        <v>45627</v>
+        <v>45566</v>
       </c>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -3667,7 +3674,7 @@
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <f t="shared" si="0"/>
-        <v>45658</v>
+        <v>45597</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -3686,7 +3693,7 @@
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <f t="shared" si="0"/>
-        <v>45689</v>
+        <v>45627</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -3705,7 +3712,7 @@
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <f t="shared" si="0"/>
-        <v>45717</v>
+        <v>45658</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -3722,7 +3729,10 @@
       <c r="K53" s="20"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="40"/>
+      <c r="A54" s="40">
+        <f t="shared" si="0"/>
+        <v>45689</v>
+      </c>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
       <c r="D54" s="39"/>
@@ -3738,7 +3748,10 @@
       <c r="K54" s="20"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="40"/>
+      <c r="A55" s="40">
+        <f t="shared" si="0"/>
+        <v>45717</v>
+      </c>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
       <c r="D55" s="39"/>
@@ -4986,34 +4999,66 @@
       <c r="K132" s="20"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A133" s="41"/>
-      <c r="B133" s="15"/>
-      <c r="C133" s="42"/>
-      <c r="D133" s="43"/>
+      <c r="A133" s="40"/>
+      <c r="B133" s="20"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="39"/>
       <c r="E133" s="9"/>
-      <c r="F133" s="15"/>
-      <c r="G133" s="42" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H133" s="43"/>
+      <c r="F133" s="20"/>
+      <c r="G133" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H133" s="39"/>
       <c r="I133" s="9"/>
-      <c r="J133" s="12"/>
-      <c r="K133" s="15"/>
+      <c r="J133" s="11"/>
+      <c r="K133" s="20"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A134" s="40"/>
+      <c r="B134" s="20"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="39"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="20"/>
+      <c r="G134" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H134" s="39"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="11"/>
+      <c r="K134" s="20"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A135" s="41"/>
+      <c r="B135" s="15"/>
+      <c r="C135" s="42"/>
+      <c r="D135" s="43"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="42" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H135" s="43"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="12"/>
+      <c r="K135" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>

<commit_message>
Update Leave Card 6/22/2023 5:35 PM
</commit_message>
<xml_diff>
--- a/ACERON, ANGELU.xlsx
+++ b/ACERON, ANGELU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D977A8C3-12E5-4264-8A9F-E3906E4B6942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FE65EA-0846-4E2C-9299-14AFD01E55C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>PERIOD</t>
   </si>
@@ -597,14 +597,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -614,9 +617,6 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2293,7 +2293,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2660,9 +2660,9 @@
   <dimension ref="A2:K135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A25" activePane="bottomLeft"/>
-      <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="3696" topLeftCell="A24" activePane="bottomLeft"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection pane="bottomLeft" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2692,14 +2692,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -2712,16 +2712,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="55">
         <v>44594</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -2734,16 +2734,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -2769,18 +2769,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -2866,7 +2866,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
-        <v>44594</v>
+        <v>44620</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="13">
@@ -2886,7 +2886,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
-        <v>44622</v>
+        <v>44651</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="13">
@@ -2906,7 +2906,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
-        <v>44653</v>
+        <v>44681</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="13">
@@ -2926,7 +2926,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
-        <v>44683</v>
+        <v>44712</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="13">
@@ -2946,7 +2946,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
-        <v>44714</v>
+        <v>44742</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="13">
@@ -2966,7 +2966,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
-        <v>44744</v>
+        <v>44773</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="13">
@@ -2986,7 +2986,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
-        <v>44775</v>
+        <v>44804</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="13">
@@ -3006,7 +3006,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
-        <v>44806</v>
+        <v>44834</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>47</v>
@@ -3027,7 +3027,9 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
+      <c r="A19" s="40" t="s">
+        <v>32</v>
+      </c>
       <c r="B19" s="20"/>
       <c r="C19" s="13">
         <v>1.25</v>
@@ -3046,7 +3048,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
-        <v>44835</v>
+        <v>44865</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>49</v>
@@ -3072,7 +3074,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
-        <v>44866</v>
+        <v>44895</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>49</v>
@@ -3097,7 +3099,9 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
+      <c r="A22" s="40" t="s">
+        <v>32</v>
+      </c>
       <c r="B22" s="20" t="s">
         <v>52</v>
       </c>
@@ -3120,7 +3124,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
-        <v>44896</v>
+        <v>44926</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>49</v>
@@ -3204,7 +3208,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
-        <v>44927</v>
+        <v>44957</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="13">
@@ -3224,8 +3228,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
-        <f>EDATE(A27,1)</f>
-        <v>44958</v>
+        <v>44985</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="13">
@@ -3245,8 +3248,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
-        <f t="shared" ref="A29:A55" si="0">EDATE(A28,1)</f>
-        <v>44986</v>
+        <v>45016</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>56</v>
@@ -3269,7 +3271,9 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
+      <c r="A30" s="40" t="s">
+        <v>32</v>
+      </c>
       <c r="B30" s="20" t="s">
         <v>56</v>
       </c>
@@ -3289,7 +3293,9 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
+      <c r="A31" s="40" t="s">
+        <v>32</v>
+      </c>
       <c r="B31" s="20" t="s">
         <v>56</v>
       </c>
@@ -3310,8 +3316,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
-        <f>EDATE(A29,1)</f>
-        <v>45017</v>
+        <v>45046</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>58</v>
@@ -3331,8 +3336,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
-        <f t="shared" si="0"/>
-        <v>45047</v>
+        <v>45077</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -3350,8 +3354,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
-        <f t="shared" si="0"/>
-        <v>45078</v>
+        <v>45107</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -3369,8 +3372,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
-        <f t="shared" si="0"/>
-        <v>45108</v>
+        <v>45138</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -3388,8 +3390,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="40">
-        <f t="shared" si="0"/>
-        <v>45139</v>
+        <v>45169</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -3407,8 +3408,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
-        <f t="shared" si="0"/>
-        <v>45170</v>
+        <v>45199</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -3426,8 +3426,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
-        <f t="shared" si="0"/>
-        <v>45200</v>
+        <v>45230</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -3445,8 +3444,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
-        <f t="shared" si="0"/>
-        <v>45231</v>
+        <v>45260</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -3464,8 +3462,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
-        <f t="shared" si="0"/>
-        <v>45261</v>
+        <v>45291</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -3483,8 +3480,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
-        <f t="shared" si="0"/>
-        <v>45292</v>
+        <v>45322</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -3502,8 +3498,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
-        <f t="shared" si="0"/>
-        <v>45323</v>
+        <v>45351</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -3521,8 +3516,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
-        <f t="shared" si="0"/>
-        <v>45352</v>
+        <v>45382</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -3540,8 +3534,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
-        <f t="shared" si="0"/>
-        <v>45383</v>
+        <v>45412</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -3559,8 +3552,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
-        <f t="shared" si="0"/>
-        <v>45413</v>
+        <v>45443</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -3578,8 +3570,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
-        <f t="shared" si="0"/>
-        <v>45444</v>
+        <v>45473</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -3597,8 +3588,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
-        <f t="shared" si="0"/>
-        <v>45474</v>
+        <v>45504</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -3616,8 +3606,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
-        <f t="shared" si="0"/>
-        <v>45505</v>
+        <v>45535</v>
       </c>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -3635,8 +3624,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40">
-        <f t="shared" si="0"/>
-        <v>45536</v>
+        <v>45565</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -3654,8 +3642,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
-        <f t="shared" si="0"/>
-        <v>45566</v>
+        <v>45596</v>
       </c>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -3673,8 +3660,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
-        <f t="shared" si="0"/>
-        <v>45597</v>
+        <v>45626</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -3692,8 +3678,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
-        <f t="shared" si="0"/>
-        <v>45627</v>
+        <v>45657</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -3711,8 +3696,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
-        <f t="shared" si="0"/>
-        <v>45658</v>
+        <v>45688</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -3730,8 +3714,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
-        <f t="shared" si="0"/>
-        <v>45689</v>
+        <v>45716</v>
       </c>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -3749,8 +3732,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40">
-        <f t="shared" si="0"/>
-        <v>45717</v>
+        <v>45747</v>
       </c>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -5048,17 +5030,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>

<commit_message>
Update Leave Card 8/3/2023 4:40 PM
</commit_message>
<xml_diff>
--- a/ACERON, ANGELU.xlsx
+++ b/ACERON, ANGELU.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FE65EA-0846-4E2C-9299-14AFD01E55C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <definedName name="BALANCE_1">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>PERIOD</t>
   </si>
@@ -218,7 +217,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -597,17 +596,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -617,6 +613,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -906,7 +905,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -949,7 +948,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1013,7 +1012,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1073,7 +1072,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1139,7 +1138,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1202,7 +1201,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1299,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1358,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,7 +1423,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1467,7 +1466,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1542,7 +1541,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1728,7 +1727,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1794,7 +1793,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1852,7 +1851,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1918,7 +1917,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1974,7 +1973,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2049,7 +2048,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2092,7 +2091,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2158,7 +2157,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2214,7 +2213,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2293,7 +2292,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2310,25 +2309,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K135" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K135" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2635,7 +2634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2645,7 +2644,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2653,34 +2652,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A24" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A24" activePane="bottomLeft"/>
       <selection activeCell="L1" sqref="L1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="N32" sqref="N32"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -2692,16 +2691,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -2712,18 +2711,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>44594</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -2734,18 +2733,18 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -2753,7 +2752,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -2766,24 +2765,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -2818,7 +2817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -2827,7 +2826,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>6.2079999999999984</v>
+        <v>8.9579999999999984</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2837,12 +2836,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>16.207999999999998</v>
+        <v>19.957999999999998</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>46</v>
       </c>
@@ -2864,7 +2863,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>44620</v>
       </c>
@@ -2884,7 +2883,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>44651</v>
       </c>
@@ -2904,7 +2903,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>44681</v>
       </c>
@@ -2924,7 +2923,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>44712</v>
       </c>
@@ -2944,7 +2943,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>44742</v>
       </c>
@@ -2964,7 +2963,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>44773</v>
       </c>
@@ -2984,7 +2983,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>44804</v>
       </c>
@@ -3004,7 +3003,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>44834</v>
       </c>
@@ -3026,7 +3025,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>32</v>
       </c>
@@ -3046,7 +3045,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>44865</v>
       </c>
@@ -3072,7 +3071,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>44895</v>
       </c>
@@ -3098,7 +3097,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
         <v>32</v>
       </c>
@@ -3122,7 +3121,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>44926</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="20" t="s">
         <v>56</v>
@@ -3166,7 +3165,7 @@
         <v>44918</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="20" t="s">
         <v>57</v>
@@ -3188,7 +3187,7 @@
         <v>44923</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>54</v>
       </c>
@@ -3206,7 +3205,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>44957</v>
       </c>
@@ -3226,7 +3225,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>44985</v>
       </c>
@@ -3246,7 +3245,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>45016</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
         <v>32</v>
       </c>
@@ -3292,7 +3291,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>32</v>
       </c>
@@ -3314,69 +3313,79 @@
         <v>45013</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>45046</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D32" s="39"/>
       <c r="E32" s="9"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G32" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H32" s="39"/>
       <c r="I32" s="9"/>
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>45077</v>
       </c>
       <c r="B33" s="20"/>
-      <c r="C33" s="13"/>
+      <c r="C33" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D33" s="39"/>
       <c r="E33" s="9"/>
       <c r="F33" s="20"/>
-      <c r="G33" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G33" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H33" s="39"/>
       <c r="I33" s="9"/>
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>45107</v>
       </c>
       <c r="B34" s="20"/>
-      <c r="C34" s="13"/>
+      <c r="C34" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D34" s="39"/>
       <c r="E34" s="9"/>
       <c r="F34" s="20"/>
-      <c r="G34" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G34" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H34" s="39"/>
       <c r="I34" s="9"/>
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>45138</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="C35" s="13"/>
-      <c r="D35" s="39"/>
+      <c r="D35" s="39">
+        <v>1</v>
+      </c>
       <c r="E35" s="9"/>
       <c r="F35" s="20"/>
       <c r="G35" s="13" t="str">
@@ -3386,9 +3395,11 @@
       <c r="H35" s="39"/>
       <c r="I35" s="9"/>
       <c r="J35" s="11"/>
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K35" s="49">
+        <v>45127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40">
         <v>45169</v>
       </c>
@@ -3406,7 +3417,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>45199</v>
       </c>
@@ -3424,7 +3435,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>45230</v>
       </c>
@@ -3442,7 +3453,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>45260</v>
       </c>
@@ -3460,7 +3471,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>45291</v>
       </c>
@@ -3478,7 +3489,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>45322</v>
       </c>
@@ -3496,7 +3507,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <v>45351</v>
       </c>
@@ -3514,7 +3525,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>45382</v>
       </c>
@@ -3532,7 +3543,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>45412</v>
       </c>
@@ -3550,7 +3561,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>45443</v>
       </c>
@@ -3568,7 +3579,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>45473</v>
       </c>
@@ -3586,7 +3597,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>45504</v>
       </c>
@@ -3604,7 +3615,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>45535</v>
       </c>
@@ -3622,7 +3633,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40">
         <v>45565</v>
       </c>
@@ -3640,7 +3651,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40">
         <v>45596</v>
       </c>
@@ -3658,7 +3669,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
         <v>45626</v>
       </c>
@@ -3676,7 +3687,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
         <v>45657</v>
       </c>
@@ -3694,7 +3705,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
         <v>45688</v>
       </c>
@@ -3712,7 +3723,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40">
         <v>45716</v>
       </c>
@@ -3730,7 +3741,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40">
         <v>45747</v>
       </c>
@@ -3748,7 +3759,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -3764,7 +3775,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -3780,7 +3791,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -3796,7 +3807,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -3812,7 +3823,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -3828,7 +3839,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -3844,7 +3855,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -3860,7 +3871,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -3876,7 +3887,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -3892,7 +3903,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -3908,7 +3919,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -3924,7 +3935,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -3940,7 +3951,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -3956,7 +3967,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -3972,7 +3983,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -3988,7 +3999,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -4004,7 +4015,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -4020,7 +4031,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -4036,7 +4047,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -4052,7 +4063,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4068,7 +4079,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4084,7 +4095,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4100,7 +4111,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4116,7 +4127,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4132,7 +4143,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4148,7 +4159,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4164,7 +4175,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4180,7 +4191,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4196,7 +4207,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4212,7 +4223,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4228,7 +4239,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4244,7 +4255,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4260,7 +4271,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4276,7 +4287,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4292,7 +4303,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4308,7 +4319,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4324,7 +4335,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4340,7 +4351,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4356,7 +4367,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4372,7 +4383,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4388,7 +4399,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4404,7 +4415,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4420,7 +4431,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4436,7 +4447,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4452,7 +4463,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4468,7 +4479,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4484,7 +4495,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4500,7 +4511,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4516,7 +4527,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4532,7 +4543,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4548,7 +4559,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4564,7 +4575,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4580,7 +4591,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4596,7 +4607,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4612,7 +4623,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4628,7 +4639,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4644,7 +4655,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4660,7 +4671,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4676,7 +4687,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4692,7 +4703,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4708,7 +4719,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4724,7 +4735,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4740,7 +4751,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4756,7 +4767,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4772,7 +4783,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -4788,7 +4799,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -4804,7 +4815,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -4820,7 +4831,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -4836,7 +4847,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -4852,7 +4863,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -4868,7 +4879,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -4884,7 +4895,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -4900,7 +4911,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -4916,7 +4927,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -4932,7 +4943,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -4948,7 +4959,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -4964,7 +4975,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -4980,7 +4991,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -4996,7 +5007,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="40"/>
       <c r="B134" s="20"/>
       <c r="C134" s="13"/>
@@ -5012,7 +5023,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="41"/>
       <c r="B135" s="15"/>
       <c r="C135" s="42"/>
@@ -5030,23 +5041,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5069,28 +5080,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5103,7 +5114,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5132,7 +5143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3" s="11"/>
@@ -5154,17 +5165,17 @@
         <v>1.208</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5185,7 +5196,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5212,7 +5223,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5238,7 +5249,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5264,7 +5275,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5290,7 +5301,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5316,7 +5327,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5342,7 +5353,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5368,7 +5379,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5394,7 +5405,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5414,7 +5425,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5434,7 +5445,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5454,7 +5465,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5475,7 +5486,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5496,7 +5507,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5517,7 +5528,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5538,7 +5549,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5559,7 +5570,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5580,7 +5591,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -5601,7 +5612,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -5622,7 +5633,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -5643,7 +5654,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -5664,7 +5675,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -5685,7 +5696,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -5706,7 +5717,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -5727,7 +5738,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -5748,7 +5759,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -5769,7 +5780,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -5790,7 +5801,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -5811,7 +5822,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -5832,7 +5843,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -5853,7 +5864,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -5874,7 +5885,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -5883,7 +5894,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -5892,7 +5903,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -5901,7 +5912,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -5910,7 +5921,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -5919,7 +5930,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -5928,7 +5939,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -5937,7 +5948,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -5946,7 +5957,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -5955,7 +5966,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -5964,7 +5975,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -5973,7 +5984,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -5982,7 +5993,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -5991,7 +6002,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6000,7 +6011,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6009,7 +6020,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6018,7 +6029,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6027,7 +6038,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6036,7 +6047,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6045,7 +6056,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6054,7 +6065,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6063,7 +6074,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6072,7 +6083,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6081,7 +6092,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6090,7 +6101,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6099,7 +6110,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6108,7 +6119,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6117,7 +6128,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6126,7 +6137,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6135,7 +6146,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
Add Leave Card 10/32023 3:18 PM
</commit_message>
<xml_diff>
--- a/ACERON, ANGELU.xlsx
+++ b/ACERON, ANGELU.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>PERIOD</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SL(1-0-0)</t>
+  </si>
+  <si>
+    <t>FL(1-0-0)</t>
   </si>
 </sst>
 </file>
@@ -2309,7 +2315,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K135" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K137" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
@@ -2656,12 +2662,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K135"/>
+  <dimension ref="A2:K137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A24" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A27" activePane="bottomLeft"/>
       <selection activeCell="L1" sqref="L1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,7 +2832,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>8.9579999999999984</v>
+        <v>8.7079999999999984</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2836,7 +2842,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>19.957999999999998</v>
+        <v>22.707999999999998</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -3382,15 +3388,17 @@
       <c r="B35" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D35" s="39">
         <v>1</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="20"/>
-      <c r="G35" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G35" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H35" s="39"/>
       <c r="I35" s="9"/>
@@ -3403,27 +3411,37 @@
       <c r="A36" s="40">
         <v>45169</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D36" s="39"/>
       <c r="E36" s="9"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H36" s="39"/>
+      <c r="G36" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H36" s="39">
+        <v>1</v>
+      </c>
       <c r="I36" s="9"/>
       <c r="J36" s="11"/>
-      <c r="K36" s="20"/>
+      <c r="K36" s="49">
+        <v>45137</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="40">
-        <v>45199</v>
-      </c>
-      <c r="B37" s="20"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="C37" s="13"/>
-      <c r="D37" s="39"/>
+      <c r="D37" s="39">
+        <v>1</v>
+      </c>
       <c r="E37" s="9"/>
       <c r="F37" s="20"/>
       <c r="G37" s="13" t="str">
@@ -3433,33 +3451,47 @@
       <c r="H37" s="39"/>
       <c r="I37" s="9"/>
       <c r="J37" s="11"/>
-      <c r="K37" s="20"/>
+      <c r="K37" s="49">
+        <v>45168</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
-        <v>45230</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="39"/>
+        <v>45199</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D38" s="39">
+        <v>1</v>
+      </c>
       <c r="E38" s="9"/>
       <c r="F38" s="20"/>
-      <c r="G38" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G38" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H38" s="39"/>
       <c r="I38" s="9"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="20"/>
+      <c r="K38" s="49">
+        <v>45182</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
-        <v>45260</v>
-      </c>
-      <c r="B39" s="20"/>
+        <v>45230</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="C39" s="13"/>
-      <c r="D39" s="39"/>
+      <c r="D39" s="39">
+        <v>1</v>
+      </c>
       <c r="E39" s="9"/>
       <c r="F39" s="20"/>
       <c r="G39" s="13" t="str">
@@ -3469,15 +3501,19 @@
       <c r="H39" s="39"/>
       <c r="I39" s="9"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="20"/>
+      <c r="K39" s="49">
+        <v>45195</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="40">
-        <v>45291</v>
-      </c>
-      <c r="B40" s="20"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="C40" s="13"/>
-      <c r="D40" s="39"/>
+      <c r="D40" s="39">
+        <v>1</v>
+      </c>
       <c r="E40" s="9"/>
       <c r="F40" s="20"/>
       <c r="G40" s="13" t="str">
@@ -3487,11 +3523,13 @@
       <c r="H40" s="39"/>
       <c r="I40" s="9"/>
       <c r="J40" s="11"/>
-      <c r="K40" s="20"/>
+      <c r="K40" s="49">
+        <v>45203</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
-        <v>45322</v>
+        <v>45260</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -3509,7 +3547,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
-        <v>45351</v>
+        <v>45291</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -3527,7 +3565,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
-        <v>45382</v>
+        <v>45322</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -3545,7 +3583,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
-        <v>45412</v>
+        <v>45351</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -3563,7 +3601,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
-        <v>45443</v>
+        <v>45382</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -3581,7 +3619,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
-        <v>45473</v>
+        <v>45412</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -3599,7 +3637,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
-        <v>45504</v>
+        <v>45443</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -3617,7 +3655,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
-        <v>45535</v>
+        <v>45473</v>
       </c>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -3635,7 +3673,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40">
-        <v>45565</v>
+        <v>45504</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -3653,7 +3691,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40">
-        <v>45596</v>
+        <v>45535</v>
       </c>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -3671,7 +3709,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
-        <v>45626</v>
+        <v>45565</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -3689,7 +3727,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
-        <v>45657</v>
+        <v>45596</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -3707,7 +3745,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
-        <v>45688</v>
+        <v>45626</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -3725,7 +3763,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40">
-        <v>45716</v>
+        <v>45657</v>
       </c>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -3743,7 +3781,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40">
-        <v>45747</v>
+        <v>45688</v>
       </c>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -3760,7 +3798,9 @@
       <c r="K55" s="20"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="40"/>
+      <c r="A56" s="40">
+        <v>45716</v>
+      </c>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
       <c r="D56" s="39"/>
@@ -3776,7 +3816,9 @@
       <c r="K56" s="20"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="40"/>
+      <c r="A57" s="40">
+        <v>45747</v>
+      </c>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
       <c r="D57" s="39"/>
@@ -5024,20 +5066,52 @@
       <c r="K134" s="20"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="41"/>
-      <c r="B135" s="15"/>
-      <c r="C135" s="42"/>
-      <c r="D135" s="43"/>
+      <c r="A135" s="40"/>
+      <c r="B135" s="20"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="39"/>
       <c r="E135" s="9"/>
-      <c r="F135" s="15"/>
-      <c r="G135" s="42" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H135" s="43"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H135" s="39"/>
       <c r="I135" s="9"/>
-      <c r="J135" s="12"/>
-      <c r="K135" s="15"/>
+      <c r="J135" s="11"/>
+      <c r="K135" s="20"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136" s="40"/>
+      <c r="B136" s="20"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="39"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="20"/>
+      <c r="G136" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H136" s="39"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="11"/>
+      <c r="K136" s="20"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137" s="41"/>
+      <c r="B137" s="15"/>
+      <c r="C137" s="42"/>
+      <c r="D137" s="43"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="42" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H137" s="43"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="12"/>
+      <c r="K137" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5053,7 +5127,7 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
@@ -5062,7 +5136,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="89" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"&amp;12REPUBLIC OF THE PHILIPPINES
 CITY OF TAGAYTAY
@@ -5070,8 +5144,8 @@
     <oddFooter>&amp;L
 PREPARED BY: ___________________
 DATE: &amp;D, &amp;T&amp;C
-CERTIFIED CORRECT BY: &amp;UALMA A. MALABANAN&amp;U
-                                   HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
+CERTIFIED CORRECT BY: &amp;UNANETTE B. SUSA&amp;U
+                                                    OIC - HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>